<commit_message>
Aula12 - 19/09 - FPA
</commit_message>
<xml_diff>
--- a/FerramentaFPAProfRJPManual.xlsx
+++ b/FerramentaFPAProfRJPManual.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\labsfiap\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\Governanca-e-Melhores-Praticas-em-TI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99FB4411-1EAD-43EC-BD98-D986A9DD1BA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFF41924-B39D-4AE0-9B69-CDE7D5E9CEF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="83">
   <si>
     <t>COMPONENTE FUNCIONAL BÁSICO (CFB)</t>
   </si>
@@ -255,6 +255,36 @@
   </si>
   <si>
     <t>Registro de tipos de chamados</t>
+  </si>
+  <si>
+    <t>Id contrato; Data validade; Status pagamento; Cnpj cliente; Flag suporte autorizado</t>
+  </si>
+  <si>
+    <t>Id protocolo; Nome cliente; Telefone contato cliente; Email cliente; Id analista; Data de inclusão; Descrição do problema; Data início do problema; Prioridade; Tipo do chamado; Data solução; Descrição da solução</t>
+  </si>
+  <si>
+    <t>Palavra chave; Tipo</t>
+  </si>
+  <si>
+    <t>Palavra chave; Prioridade</t>
+  </si>
+  <si>
+    <t>Id contrato; Flag suporte contrato</t>
+  </si>
+  <si>
+    <t>Id protocolo; Nome cliente; Telefone contato cliente; Email cliente; Id analista; Data de inclusão; Descrição do problema; Data início do problema; Prioridade; Tipo do chamado;</t>
+  </si>
+  <si>
+    <t>Id protocolo; Nome cliente; Telefone contato cliente; Email cliente; Data de inclusão; Descrição do problema; Data início do problema; Prioridade; Tipo do chamado;</t>
+  </si>
+  <si>
+    <t>Id protocolo; Data de inclusão; Prioridade; Tipo do chamado;</t>
+  </si>
+  <si>
+    <t>Descrição do problema; Palavra chave; Tipo do chamado</t>
+  </si>
+  <si>
+    <t>Descrição do problema; Palavra chave; Prioridade</t>
   </si>
 </sst>
 </file>
@@ -1470,7 +1500,7 @@
   <dimension ref="A1:H240"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1568,7 +1598,7 @@
       <c r="G9" s="30"/>
       <c r="H9" s="30"/>
     </row>
-    <row r="10" spans="1:8" s="31" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" s="31" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="32" t="s">
         <v>57</v>
       </c>
@@ -1581,8 +1611,12 @@
       <c r="D10" s="30">
         <v>1</v>
       </c>
-      <c r="E10" s="32"/>
-      <c r="F10" s="30"/>
+      <c r="E10" s="32" t="s">
+        <v>73</v>
+      </c>
+      <c r="F10" s="30">
+        <v>5</v>
+      </c>
       <c r="G10" s="33"/>
       <c r="H10" s="30"/>
     </row>
@@ -1599,12 +1633,16 @@
       <c r="D11" s="30">
         <v>1</v>
       </c>
-      <c r="E11" s="32"/>
-      <c r="F11" s="30"/>
+      <c r="E11" s="32" t="s">
+        <v>77</v>
+      </c>
+      <c r="F11" s="30">
+        <v>2</v>
+      </c>
       <c r="G11" s="33"/>
       <c r="H11" s="30"/>
     </row>
-    <row r="12" spans="1:8" s="31" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" s="31" customFormat="1" ht="120" x14ac:dyDescent="0.25">
       <c r="A12" s="32" t="s">
         <v>59</v>
       </c>
@@ -1617,12 +1655,16 @@
       <c r="D12" s="30">
         <v>1</v>
       </c>
-      <c r="E12" s="32"/>
-      <c r="F12" s="30"/>
+      <c r="E12" s="32" t="s">
+        <v>74</v>
+      </c>
+      <c r="F12" s="30">
+        <v>12</v>
+      </c>
       <c r="G12" s="33"/>
       <c r="H12" s="30"/>
     </row>
-    <row r="13" spans="1:8" s="31" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" s="31" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A13" s="32" t="s">
         <v>60</v>
       </c>
@@ -1635,12 +1677,16 @@
       <c r="D13" s="30">
         <v>1</v>
       </c>
-      <c r="E13" s="32"/>
-      <c r="F13" s="30"/>
+      <c r="E13" s="32" t="s">
+        <v>78</v>
+      </c>
+      <c r="F13" s="30">
+        <v>10</v>
+      </c>
       <c r="G13" s="33"/>
       <c r="H13" s="30"/>
     </row>
-    <row r="14" spans="1:8" s="31" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" s="31" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A14" s="32" t="s">
         <v>61</v>
       </c>
@@ -1651,8 +1697,12 @@
         <v>67</v>
       </c>
       <c r="D14" s="30"/>
-      <c r="E14" s="32"/>
-      <c r="F14" s="30"/>
+      <c r="E14" s="32" t="s">
+        <v>79</v>
+      </c>
+      <c r="F14" s="30">
+        <v>8</v>
+      </c>
       <c r="G14" s="33"/>
       <c r="H14" s="30"/>
     </row>
@@ -1667,12 +1717,16 @@
         <v>67</v>
       </c>
       <c r="D15" s="30"/>
-      <c r="E15" s="32"/>
-      <c r="F15" s="30"/>
+      <c r="E15" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="F15" s="30">
+        <v>4</v>
+      </c>
       <c r="G15" s="33"/>
       <c r="H15" s="30"/>
     </row>
-    <row r="16" spans="1:8" s="31" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" s="31" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="32" t="s">
         <v>63</v>
       </c>
@@ -1685,12 +1739,16 @@
       <c r="D16" s="30">
         <v>1</v>
       </c>
-      <c r="E16" s="32"/>
-      <c r="F16" s="30"/>
+      <c r="E16" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="F16" s="30">
+        <v>4</v>
+      </c>
       <c r="G16" s="33"/>
       <c r="H16" s="30"/>
     </row>
-    <row r="17" spans="1:8" s="31" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" s="31" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="32" t="s">
         <v>64</v>
       </c>
@@ -1703,12 +1761,16 @@
       <c r="D17" s="30">
         <v>1</v>
       </c>
-      <c r="E17" s="32"/>
-      <c r="F17" s="30"/>
+      <c r="E17" s="32" t="s">
+        <v>81</v>
+      </c>
+      <c r="F17" s="30">
+        <v>3</v>
+      </c>
       <c r="G17" s="33"/>
       <c r="H17" s="30"/>
     </row>
-    <row r="18" spans="1:8" s="31" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" s="31" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="32" t="s">
         <v>65</v>
       </c>
@@ -1721,8 +1783,12 @@
       <c r="D18" s="30">
         <v>1</v>
       </c>
-      <c r="E18" s="32"/>
-      <c r="F18" s="30"/>
+      <c r="E18" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="F18" s="30">
+        <v>3</v>
+      </c>
       <c r="G18" s="33"/>
       <c r="H18" s="30"/>
     </row>
@@ -1739,8 +1805,12 @@
       <c r="D19" s="30">
         <v>1</v>
       </c>
-      <c r="E19" s="32"/>
-      <c r="F19" s="30"/>
+      <c r="E19" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="F19" s="30">
+        <v>2</v>
+      </c>
       <c r="G19" s="33"/>
       <c r="H19" s="30"/>
     </row>
@@ -1757,8 +1827,12 @@
       <c r="D20" s="30">
         <v>1</v>
       </c>
-      <c r="E20" s="32"/>
-      <c r="F20" s="30"/>
+      <c r="E20" s="32" t="s">
+        <v>75</v>
+      </c>
+      <c r="F20" s="30">
+        <v>2</v>
+      </c>
       <c r="G20" s="33"/>
       <c r="H20" s="30"/>
     </row>
@@ -3968,7 +4042,7 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
           <x14:formula1>
             <xm:f>Seletores!$A$2:$A$6</xm:f>
@@ -3991,7 +4065,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -7280,7 +7356,7 @@
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O7" sqref="O7"/>
+      <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>